<commit_message>
fixed: rm script file
</commit_message>
<xml_diff>
--- a/hokaidovietnam_backend/phân tích .xlsx
+++ b/hokaidovietnam_backend/phân tích .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tan\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A8B2A9-3095-444E-B2EB-451D973A53A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D0E5BE-20B5-4DCC-A5ED-7C6F316BFD09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1753" yWindow="-10205" windowWidth="22627" windowHeight="9391" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13148" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="63">
   <si>
     <t>user</t>
   </si>
@@ -90,9 +90,6 @@
     <t>id fk</t>
   </si>
   <si>
-    <t>user_id_PK</t>
-  </si>
-  <si>
     <t>sp</t>
   </si>
   <si>
@@ -168,14 +165,74 @@
     <t>Thành_tiền</t>
   </si>
   <si>
-    <t>user_id Fk</t>
+    <t>Email_PK</t>
+  </si>
+  <si>
+    <t>Email_Fk</t>
+  </si>
+  <si>
+    <t>soDt</t>
+  </si>
+  <si>
+    <t>GioHang</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>nguoi_dung_id</t>
+  </si>
+  <si>
+    <t>san_pham_id</t>
+  </si>
+  <si>
+    <t>so_luong</t>
+  </si>
+  <si>
+    <t>chưa gọi</t>
+  </si>
+  <si>
+    <t>toi can mua hang</t>
+  </si>
+  <si>
+    <t>abcd@</t>
+  </si>
+  <si>
+    <t>nhut</t>
+  </si>
+  <si>
+    <t>spam</t>
+  </si>
+  <si>
+    <t>đã gọi</t>
+  </si>
+  <si>
+    <t>hh</t>
+  </si>
+  <si>
+    <t>kkkk</t>
+  </si>
+  <si>
+    <t>trang_thai</t>
+  </si>
+  <si>
+    <t>noi_dung</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>ho_ten</t>
+  </si>
+  <si>
+    <t>Liên hệ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,8 +260,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,6 +301,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -242,10 +347,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -260,12 +366,28 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -608,611 +730,942 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3F8F735-820D-4089-B5C0-69A0D2D025D0}">
-  <dimension ref="A1:R35"/>
+  <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="3"/>
-    <col min="8" max="8" width="8.88671875" style="2"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="3"/>
+    <col min="9" max="9" width="8.88671875" style="2"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.33203125" customWidth="1"/>
+    <col min="18" max="18" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="D1" s="8"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="R4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="R4" s="4" t="s">
+      <c r="S4" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="Q5" s="4">
+        <v>1</v>
+      </c>
+      <c r="R5" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="P5" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="R5" s="4">
+      <c r="S5" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9"/>
       <c r="F6" s="8"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="8" t="s">
+      <c r="G6" s="8"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="8"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
-      <c r="P6" s="4">
-        <v>2</v>
-      </c>
-      <c r="Q6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="R6" s="4">
+      <c r="N6" s="8"/>
+      <c r="Q6" s="4">
+        <v>2</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="S6" s="4">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="I7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>3</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="S7" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8" s="14">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4">
+        <v>2</v>
+      </c>
+      <c r="C8" s="4">
+        <v>909240886</v>
+      </c>
+      <c r="D8" s="7">
+        <v>45368</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="4" t="s">
+      <c r="F8" s="4">
+        <v>85</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
+      <c r="I8" s="6">
+        <v>1</v>
+      </c>
+      <c r="J8" s="11">
+        <v>1</v>
+      </c>
+      <c r="K8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="4" t="s">
+      <c r="L8" s="4">
+        <v>10</v>
+      </c>
+      <c r="M8" s="4">
+        <v>5</v>
+      </c>
+      <c r="N8" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" s="15">
+        <v>2</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4">
+        <v>918777666</v>
+      </c>
+      <c r="D9" s="7">
+        <v>45369</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="4">
+        <v>180</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
+      <c r="I9" s="6">
+        <v>2</v>
+      </c>
+      <c r="J9" s="11">
+        <v>1</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="4">
+        <v>5</v>
+      </c>
+      <c r="M9" s="4">
+        <v>7</v>
+      </c>
+      <c r="N9" s="4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10" s="16">
+        <v>3</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4">
+        <v>909240886</v>
+      </c>
+      <c r="D10" s="7">
+        <v>45370</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="4">
+        <v>630</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1</v>
+      </c>
+      <c r="I10" s="6">
+        <v>3</v>
+      </c>
+      <c r="J10" s="13">
+        <v>2</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="4">
         <v>20</v>
       </c>
-      <c r="L7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="M7" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="P7" s="4">
-        <v>3</v>
-      </c>
-      <c r="Q7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="R7" s="4">
+      <c r="M10" s="4">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
-        <v>1</v>
-      </c>
-      <c r="B8" s="4">
-        <v>2</v>
-      </c>
-      <c r="C8" s="7">
-        <v>45368</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="4">
-        <v>85</v>
-      </c>
-      <c r="F8" s="4">
-        <v>1</v>
-      </c>
-      <c r="H8" s="6">
-        <v>1</v>
-      </c>
-      <c r="I8" s="4">
-        <v>1</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K8" s="4">
-        <v>10</v>
-      </c>
-      <c r="L8" s="4">
-        <v>5</v>
-      </c>
-      <c r="M8" s="4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
-        <v>2</v>
-      </c>
-      <c r="B9" s="4">
-        <v>1</v>
-      </c>
-      <c r="C9" s="7">
-        <v>45369</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="4">
+      <c r="N10" s="4">
         <v>180</v>
       </c>
-      <c r="F9" s="4">
-        <v>1</v>
-      </c>
-      <c r="H9" s="6">
-        <v>2</v>
-      </c>
-      <c r="I9" s="4">
-        <v>1</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K9" s="4">
-        <v>5</v>
-      </c>
-      <c r="L9" s="4">
-        <v>7</v>
-      </c>
-      <c r="M9" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="6">
-        <v>3</v>
-      </c>
-      <c r="B10" s="4">
-        <v>1</v>
-      </c>
-      <c r="C10" s="7">
-        <v>45370</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="4">
-        <v>630</v>
-      </c>
-      <c r="F10" s="4">
-        <v>1</v>
-      </c>
-      <c r="H10" s="6">
-        <v>3</v>
-      </c>
-      <c r="I10" s="4">
-        <v>2</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K10" s="4">
-        <v>20</v>
-      </c>
-      <c r="L10" s="4">
-        <v>9</v>
-      </c>
-      <c r="M10" s="4">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P10" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>4</v>
       </c>
       <c r="B11" s="4"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="5"/>
       <c r="F11" s="4"/>
-      <c r="H11" s="6">
+      <c r="G11" s="4"/>
+      <c r="I11" s="6">
         <v>4</v>
       </c>
-      <c r="I11" s="4">
+      <c r="J11" s="12">
         <v>3</v>
       </c>
-      <c r="J11" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K11" s="4">
+      <c r="K11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L11" s="4">
         <v>30</v>
       </c>
-      <c r="L11" s="4">
+      <c r="M11" s="4">
         <v>5</v>
       </c>
-      <c r="M11" s="4">
+      <c r="N11" s="4">
         <v>150</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="T11" s="4"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="5"/>
       <c r="F12" s="4"/>
-      <c r="H12" s="6">
+      <c r="G12" s="4"/>
+      <c r="I12" s="6">
         <v>5</v>
       </c>
-      <c r="I12" s="4">
+      <c r="J12" s="12">
         <v>3</v>
       </c>
-      <c r="J12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K12" s="4">
+      <c r="K12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" s="4">
         <v>30</v>
       </c>
-      <c r="L12" s="4">
+      <c r="M12" s="4">
         <v>7</v>
       </c>
-      <c r="M12" s="4">
+      <c r="N12" s="4">
         <v>210</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P12" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>2</v>
+      </c>
+      <c r="R12" s="4">
+        <v>1</v>
+      </c>
+      <c r="S12" s="4">
+        <v>2</v>
+      </c>
+      <c r="T12" s="4"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>6</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5"/>
       <c r="F13" s="4"/>
-      <c r="H13" s="6">
+      <c r="G13" s="4"/>
+      <c r="I13" s="6">
         <v>6</v>
       </c>
-      <c r="I13" s="4">
+      <c r="J13" s="12">
         <v>3</v>
       </c>
-      <c r="J13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K13" s="4">
+      <c r="K13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" s="4">
         <v>30</v>
       </c>
-      <c r="L13" s="4">
+      <c r="M13" s="4">
         <v>9</v>
       </c>
-      <c r="M13" s="4">
+      <c r="N13" s="4">
         <v>270</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>7</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="5"/>
       <c r="F14" s="4"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="I14" s="6"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="H15" s="6"/>
-      <c r="I15" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="I15" s="6"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="H16" s="6"/>
-      <c r="I16" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="I16" s="6"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
-    </row>
-    <row r="17" spans="8:13" x14ac:dyDescent="0.3">
-      <c r="H17" s="6"/>
-      <c r="I17" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+    </row>
+    <row r="17" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="I17" s="6"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
-    </row>
-    <row r="18" spans="8:13" x14ac:dyDescent="0.3">
-      <c r="H18" s="6"/>
-      <c r="I18" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+    </row>
+    <row r="18" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="I18" s="6"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
-    </row>
-    <row r="19" spans="8:13" x14ac:dyDescent="0.3">
-      <c r="H19" s="6"/>
-      <c r="I19" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+    </row>
+    <row r="19" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="I19" s="6"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
-    </row>
-    <row r="22" spans="8:13" x14ac:dyDescent="0.3">
-      <c r="I22" t="s">
+      <c r="N19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+    </row>
+    <row r="20" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C20" s="4">
+        <v>909240886</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20" s="3">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="21" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C21" s="4">
+        <v>918777666</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="3">
+        <v>180</v>
+      </c>
+      <c r="O21" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+    </row>
+    <row r="22" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="J22" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="8:13" x14ac:dyDescent="0.3">
-      <c r="H23" s="2" t="s">
+      <c r="O22" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="P22" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q22" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="R22" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="S22" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="I23" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="8:13" x14ac:dyDescent="0.3">
-      <c r="H24" s="2">
-        <v>1</v>
-      </c>
-      <c r="I24">
+      <c r="O23" s="17">
+        <v>1</v>
+      </c>
+      <c r="P23" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q23" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="R23" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="S23" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="I24" s="2">
         <v>1</v>
       </c>
       <c r="J24">
         <v>1</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24" t="s">
         <v>14</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="8:13" x14ac:dyDescent="0.3">
-      <c r="H25" s="2">
-        <v>2</v>
-      </c>
-      <c r="I25">
-        <v>1</v>
+      <c r="O24" s="17">
+        <v>2</v>
+      </c>
+      <c r="P24" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q24" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="R24" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="S24" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="I25" s="2">
+        <v>2</v>
       </c>
       <c r="J25">
-        <v>2</v>
-      </c>
-      <c r="K25" t="s">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>2</v>
+      </c>
+      <c r="L25" t="s">
         <v>14</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="26" spans="8:13" x14ac:dyDescent="0.3">
-      <c r="H26" s="2">
+      <c r="O25" s="17">
         <v>3</v>
       </c>
-      <c r="I26">
-        <v>1</v>
+      <c r="P25" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q25" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="R25" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="S25" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="I26" s="2">
+        <v>3</v>
       </c>
       <c r="J26">
         <v>1</v>
       </c>
-      <c r="K26" t="s">
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26" t="s">
         <v>14</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="27" spans="8:13" x14ac:dyDescent="0.3">
-      <c r="H27" s="2">
+      <c r="O26" s="4">
         <v>4</v>
       </c>
-      <c r="I27">
-        <v>1</v>
+      <c r="P26" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q26" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="R26" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="S26" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="I27" s="2">
+        <v>4</v>
       </c>
       <c r="J27">
         <v>1</v>
       </c>
-      <c r="K27" t="s">
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27" t="s">
         <v>14</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="8:13" x14ac:dyDescent="0.3">
-      <c r="H28" s="2">
+      <c r="O27" s="4">
         <v>5</v>
       </c>
-      <c r="I28">
-        <v>1</v>
-      </c>
-      <c r="K28" t="s">
+      <c r="P27" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q27" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="R27" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="S27" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="I28" s="2">
+        <v>5</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="L28" t="s">
         <v>14</v>
       </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="29" spans="8:13" x14ac:dyDescent="0.3">
-      <c r="H29" s="2">
+      <c r="O28" s="4">
         <v>6</v>
       </c>
-      <c r="I29">
-        <v>2</v>
-      </c>
-      <c r="K29" t="s">
+      <c r="P28" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q28" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="R28" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="S28" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="I29" s="2">
+        <v>6</v>
+      </c>
+      <c r="J29">
+        <v>2</v>
+      </c>
+      <c r="L29" t="s">
         <v>14</v>
       </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="30" spans="8:13" x14ac:dyDescent="0.3">
-      <c r="H30" s="2">
+      <c r="O29" s="4">
         <v>7</v>
       </c>
-      <c r="I30">
-        <v>2</v>
-      </c>
-      <c r="K30" t="s">
+      <c r="P29" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q29" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="R29" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="S29" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="I30" s="2">
+        <v>7</v>
+      </c>
+      <c r="J30">
+        <v>2</v>
+      </c>
+      <c r="L30" t="s">
         <v>14</v>
       </c>
-      <c r="L30" t="s">
+      <c r="M30" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="31" spans="8:13" x14ac:dyDescent="0.3">
-      <c r="H31" s="2">
+      <c r="O30" s="4">
         <v>8</v>
       </c>
-      <c r="I31">
-        <v>2</v>
-      </c>
-      <c r="K31" t="s">
+      <c r="P30" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q30" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="R30" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="S30" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="I31" s="2">
+        <v>8</v>
+      </c>
+      <c r="J31">
+        <v>2</v>
+      </c>
+      <c r="L31" t="s">
         <v>14</v>
       </c>
-      <c r="L31" t="s">
+      <c r="M31" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="32" spans="8:13" x14ac:dyDescent="0.3">
-      <c r="H32" s="2">
+      <c r="O31" s="4">
         <v>9</v>
       </c>
-      <c r="I32">
-        <v>2</v>
-      </c>
-      <c r="K32" t="s">
+      <c r="P31" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q31" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="R31" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="S31" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="I32" s="2">
+        <v>9</v>
+      </c>
+      <c r="J32">
+        <v>2</v>
+      </c>
+      <c r="L32" t="s">
         <v>14</v>
       </c>
-      <c r="L32" t="s">
+      <c r="M32" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="33" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="H33" s="2">
+      <c r="O32" s="4">
         <v>10</v>
       </c>
-      <c r="I33">
-        <v>2</v>
-      </c>
-      <c r="K33" t="s">
+      <c r="P32" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q32" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="R32" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="S32" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="9:19" x14ac:dyDescent="0.3">
+      <c r="I33" s="2">
+        <v>10</v>
+      </c>
+      <c r="J33">
+        <v>2</v>
+      </c>
+      <c r="L33" t="s">
         <v>14</v>
       </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="34" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="H34" s="2">
+      <c r="O33" s="4">
         <v>11</v>
       </c>
-      <c r="I34">
-        <v>2</v>
-      </c>
-      <c r="K34" t="s">
+      <c r="P33" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q33" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="R33" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="S33" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="9:19" x14ac:dyDescent="0.3">
+      <c r="I34" s="2">
+        <v>11</v>
+      </c>
+      <c r="J34">
+        <v>2</v>
+      </c>
+      <c r="L34" t="s">
         <v>14</v>
       </c>
-      <c r="L34" t="s">
+      <c r="M34" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="35" spans="8:12" x14ac:dyDescent="0.3">
-      <c r="H35" s="2">
+      <c r="O34" s="4">
         <v>12</v>
       </c>
-      <c r="I35">
-        <v>2</v>
-      </c>
-      <c r="K35" t="s">
+      <c r="P34" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q34" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="R34" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="S34" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="9:19" x14ac:dyDescent="0.3">
+      <c r="I35" s="2">
+        <v>12</v>
+      </c>
+      <c r="J35">
+        <v>2</v>
+      </c>
+      <c r="L35" t="s">
         <v>14</v>
       </c>
-      <c r="L35" t="s">
+      <c r="M35" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="Q23" r:id="rId1" xr:uid="{CD8481B2-FC17-4CE0-A1EE-75224F18D937}"/>
+    <hyperlink ref="Q24" r:id="rId2" xr:uid="{606A5022-D549-462E-9DBB-27B73012E422}"/>
+    <hyperlink ref="Q25" r:id="rId3" xr:uid="{CDC9E3DA-02FB-4FB2-883C-A76C832E078B}"/>
+    <hyperlink ref="Q26" r:id="rId4" xr:uid="{566FCD5B-0291-4B12-8BC8-F8703C8C7521}"/>
+    <hyperlink ref="Q27" r:id="rId5" xr:uid="{2499E2A1-BFCE-4174-B03F-E688AF1A509C}"/>
+    <hyperlink ref="Q28" r:id="rId6" xr:uid="{F666909A-8D68-42A7-9D64-9A6489ACFF7C}"/>
+    <hyperlink ref="Q29" r:id="rId7" xr:uid="{9176350C-6B2E-45D2-A33E-951A42C1C2F4}"/>
+    <hyperlink ref="Q30" r:id="rId8" xr:uid="{A1C5D3C2-4607-4EED-A4B3-6F0AA0EDEB11}"/>
+    <hyperlink ref="Q31" r:id="rId9" xr:uid="{98F65016-47BB-466B-B523-55DB29B38E32}"/>
+    <hyperlink ref="Q32" r:id="rId10" xr:uid="{68E40579-73BD-4C59-B4C4-1657DF990160}"/>
+    <hyperlink ref="Q33" r:id="rId11" xr:uid="{48F9106F-78FC-4680-AE2F-3128B5588429}"/>
+    <hyperlink ref="Q34" r:id="rId12" xr:uid="{4F152725-21FA-4F61-B604-F0921DEF1D56}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>